<commit_message>
Pending corrections on Ren1 and Ren2
There is a discrepancy in the datasheet and the actual measured voltage hysteresis values. Increasing Ren1 and Ren2 to increase the trigger hysteresis.
</commit_message>
<xml_diff>
--- a/PCB/Can and power/EN divided calc.xlsx
+++ b/PCB/Can and power/EN divided calc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin\Documents\PlatformIO\Projects\waveshare-esp32s3-roundlcd-boilerplate\PCB\Can and power\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48B3BD77-2E42-44DD-991B-2F6B1E45663E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F50B1AD-D1C0-4DCF-B51F-86E7BD29DEC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25410" yWindow="1680" windowWidth="21465" windowHeight="17400" xr2:uid="{2567A0D3-2DA3-47D9-B2C7-7126EA924C8F}"/>
+    <workbookView xWindow="2100" yWindow="1170" windowWidth="40605" windowHeight="19710" xr2:uid="{2567A0D3-2DA3-47D9-B2C7-7126EA924C8F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -410,10 +410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F52F5A09-C579-4E41-953C-4849E3B47ADC}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -421,7 +421,7 @@
     <col min="2" max="2" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>4</v>
       </c>
@@ -429,52 +429,60 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>12.2</v>
+        <v>12.6</v>
       </c>
       <c r="D2">
         <f>1.25+D4*((1.25/D5)-0.000001)</f>
-        <v>12.266833333333333</v>
+        <v>13.6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>12</v>
+        <v>12.2</v>
       </c>
       <c r="D3">
         <f>D2-D4*0.000003</f>
-        <v>12.067333333333332</v>
+        <v>13.15</v>
+      </c>
+      <c r="I3">
+        <f>12.2*(D5/(D5+D4))</f>
+        <v>1.1090909090909091</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4">
         <f>(B2-B3)/(0.000003)</f>
-        <v>66666.666666666424</v>
+        <v>133333.33333333346</v>
       </c>
       <c r="D4" s="1">
-        <v>66500</v>
+        <v>150000</v>
+      </c>
+      <c r="I4">
+        <f>12.6*D5/(D5+D4)</f>
+        <v>1.1454545454545455</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5">
         <f>1.25/((B2-1.25)/B4+0.000001)</f>
-        <v>7564.2965204235743</v>
+        <v>14513.788098693774</v>
       </c>
       <c r="D5" s="1">
-        <v>7500</v>
+        <v>15000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>